<commit_message>
Completed PRODUCT csv file for data import
</commit_message>
<xml_diff>
--- a/Documents/Database Materials/Table SQL Files/product.xlsx
+++ b/Documents/Database Materials/Table SQL Files/product.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
   <si>
     <t>product_id</t>
   </si>
@@ -40,66 +40,6 @@
     <t>supplier_id</t>
   </si>
   <si>
-    <t>quis</t>
-  </si>
-  <si>
-    <t>lorem</t>
-  </si>
-  <si>
-    <t>vitae</t>
-  </si>
-  <si>
-    <t>posuere</t>
-  </si>
-  <si>
-    <t>aliquam</t>
-  </si>
-  <si>
-    <t>ac</t>
-  </si>
-  <si>
-    <t>quam</t>
-  </si>
-  <si>
-    <t>rutrum</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>elit</t>
-  </si>
-  <si>
-    <t>fusce</t>
-  </si>
-  <si>
-    <t>mattis</t>
-  </si>
-  <si>
-    <t>massa</t>
-  </si>
-  <si>
-    <t>hac</t>
-  </si>
-  <si>
-    <t>vestibulum</t>
-  </si>
-  <si>
-    <t>mauris</t>
-  </si>
-  <si>
-    <t>nulla</t>
-  </si>
-  <si>
-    <t>euismod</t>
-  </si>
-  <si>
-    <t>velit</t>
-  </si>
-  <si>
-    <t>duis</t>
-  </si>
-  <si>
     <t>ram.jpg</t>
   </si>
   <si>
@@ -133,15 +73,6 @@
     <t>accessory.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">2x4GB DDR3 </t>
-  </si>
-  <si>
-    <t>2x8GB DDR3</t>
-  </si>
-  <si>
-    <t>2x8GB DDR4</t>
-  </si>
-  <si>
     <t>Enterprise 4-Slot</t>
   </si>
   <si>
@@ -167,6 +98,78 @@
   </si>
   <si>
     <t>Quad-core 4.0GHz Socrates</t>
+  </si>
+  <si>
+    <t>Hummingbird 120GB SSD</t>
+  </si>
+  <si>
+    <t>Pelican 2TB HDD</t>
+  </si>
+  <si>
+    <t>Falcon 500GB SSD</t>
+  </si>
+  <si>
+    <t>XenoWare Gaming PC</t>
+  </si>
+  <si>
+    <t>AZUZ Workstation PC</t>
+  </si>
+  <si>
+    <t>Pewlett Hackard Tower PC</t>
+  </si>
+  <si>
+    <t>Tesla 650W</t>
+  </si>
+  <si>
+    <t>Franklin 650W</t>
+  </si>
+  <si>
+    <t>Faraday 450W</t>
+  </si>
+  <si>
+    <t>2x8GB DDR4 Coffee Crisp</t>
+  </si>
+  <si>
+    <t>2x8GB DDR3 KitKat</t>
+  </si>
+  <si>
+    <t>2x4GB DDR3 Nature Valley</t>
+  </si>
+  <si>
+    <t>Liberty 27" 2560x1440</t>
+  </si>
+  <si>
+    <t>Redeemer 24" 1920x1080</t>
+  </si>
+  <si>
+    <t>Rushmore 24" 1920x1080</t>
+  </si>
+  <si>
+    <t>Claymore Cherry MX Brown</t>
+  </si>
+  <si>
+    <t>Changdao Cherry MX Red</t>
+  </si>
+  <si>
+    <t>Scimitar Cherry MX Red</t>
+  </si>
+  <si>
+    <t>Rhino Optical Wired</t>
+  </si>
+  <si>
+    <t>Stag Optical Wired</t>
+  </si>
+  <si>
+    <t>Hercules Optical Wireless</t>
+  </si>
+  <si>
+    <t>Blasterman Speakers</t>
+  </si>
+  <si>
+    <t>NSA Headphones</t>
+  </si>
+  <si>
+    <t>Big Brother Webcam</t>
   </si>
 </sst>
 </file>
@@ -499,7 +502,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -551,7 +554,7 @@
         <v>23.97</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -571,13 +574,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>31.36</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -597,13 +600,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <v>42.54</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -623,13 +626,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>83.29</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -649,13 +652,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>133.44999999999999</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -675,13 +678,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>51.15</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -701,13 +704,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C8">
         <v>522.41</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -727,13 +730,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>823.43</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -753,13 +756,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>781.09</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -779,13 +782,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C11">
         <v>691.23</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -805,13 +808,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C12">
         <v>472.3</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -831,13 +834,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>763.88</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -857,13 +860,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>51.16</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E14">
         <v>5</v>
@@ -883,13 +886,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <v>82.23</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <v>5</v>
@@ -909,13 +912,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C16">
-        <v>51.66</v>
+        <v>201.66</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E16">
         <v>5</v>
@@ -935,13 +938,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C17">
-        <v>33.200000000000003</v>
+        <v>83.2</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E17">
         <v>6</v>
@@ -961,13 +964,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C18">
         <v>41.24</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E18">
         <v>6</v>
@@ -987,13 +990,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C19">
-        <v>31.94</v>
+        <v>100.94</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E19">
         <v>6</v>
@@ -1013,13 +1016,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C20">
         <v>333.42</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="E20">
         <v>7</v>
@@ -1039,13 +1042,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C21">
-        <v>203.88</v>
+        <v>403.88</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <v>7</v>
@@ -1065,13 +1068,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C22">
-        <v>243.1</v>
+        <v>343.1</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="E22">
         <v>7</v>
@@ -1091,13 +1094,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="C23">
-        <v>51.27</v>
+        <v>110.27</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E23">
         <v>8</v>
@@ -1117,13 +1120,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C24">
-        <v>61.58</v>
+        <v>150.58000000000001</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E24">
         <v>8</v>
@@ -1143,13 +1146,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C25">
-        <v>31.9</v>
+        <v>131.9</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E25">
         <v>8</v>
@@ -1169,13 +1172,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C26">
-        <v>31.61</v>
+        <v>60.61</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="E26">
         <v>9</v>
@@ -1195,13 +1198,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C27">
         <v>21.32</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="E27">
         <v>9</v>
@@ -1221,13 +1224,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C28">
-        <v>21.97</v>
+        <v>51.97</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="E28">
         <v>9</v>
@@ -1247,13 +1250,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C29">
         <v>2501.5300000000002</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="E29">
         <v>10</v>
@@ -1273,13 +1276,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>1402</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="E30">
         <v>10</v>
@@ -1299,13 +1302,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C31">
         <v>1503.13</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="E31">
         <v>10</v>
@@ -1325,13 +1328,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C32">
-        <v>12.61</v>
+        <v>32.61</v>
       </c>
       <c r="D32" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E32">
         <v>11</v>
@@ -1351,13 +1354,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C33">
         <v>23.21</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E33">
         <v>11</v>
@@ -1377,13 +1380,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="C34">
-        <v>32.29</v>
+        <v>52.29</v>
       </c>
       <c r="D34" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E34">
         <v>11</v>

</xml_diff>